<commit_message>
Agregar circulo con relaciones
</commit_message>
<xml_diff>
--- a/Relaciones.xlsx
+++ b/Relaciones.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yosua\OneDrive\Escritorio\PROYECTO FINAL VISUAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jasso\TEC\visualizacion\amazon-viz\repo\words_viewer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C693A3AF-0D38-40CA-8232-2D9622629E64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5515548D-3201-49A0-B2C3-F5E90FCF153D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{54D89E41-C334-4761-8A31-132A1CACAB93}"/>
+    <workbookView xWindow="-20520" yWindow="1695" windowWidth="20640" windowHeight="11160" xr2:uid="{54D89E41-C334-4761-8A31-132A1CACAB93}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -504,19 +504,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F772C6D-B1E8-4893-8CA4-20CDFC728D5B}">
   <dimension ref="A1:E481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A477" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A481" sqref="A481"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7265625" customWidth="1"/>
-    <col min="2" max="2" width="12.81640625" customWidth="1"/>
-    <col min="3" max="3" width="14.90625" customWidth="1"/>
-    <col min="4" max="4" width="15.6328125" customWidth="1"/>
+    <col min="1" max="1" width="35.77734375" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -533,7 +533,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -550,7 +550,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -567,7 +567,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -584,7 +584,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -601,7 +601,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -618,7 +618,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -635,7 +635,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -652,7 +652,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -669,7 +669,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -686,7 +686,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -703,7 +703,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -720,7 +720,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -737,7 +737,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -754,7 +754,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -771,7 +771,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -788,7 +788,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -805,7 +805,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -822,7 +822,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -839,7 +839,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -856,7 +856,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -873,7 +873,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -890,7 +890,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -907,7 +907,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -924,7 +924,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -941,7 +941,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -958,7 +958,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -975,7 +975,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -992,7 +992,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -1230,7 +1230,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>4</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>33</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>33</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>33</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>33</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>33</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>33</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>33</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>33</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>33</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>33</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>33</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>33</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>33</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>33</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>33</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>33</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>33</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>33</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>33</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>33</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>33</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>33</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>33</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>33</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>33</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>33</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>33</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>33</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>33</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>33</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>33</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>33</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>33</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>33</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>33</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>33</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>33</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>33</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>33</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>33</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>33</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>33</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>33</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>33</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>33</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>33</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>33</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>33</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>34</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>34</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>34</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>34</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>34</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>34</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>34</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>34</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>34</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>34</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>34</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>34</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>34</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>34</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>34</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>34</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>34</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>34</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>34</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>34</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>34</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>34</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>34</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>34</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>34</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>34</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>34</v>
       </c>
@@ -2624,7 +2624,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>34</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>34</v>
       </c>
@@ -2658,7 +2658,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>34</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>34</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>34</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>34</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>34</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>34</v>
       </c>
@@ -2760,7 +2760,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>34</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>34</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>34</v>
       </c>
@@ -2811,7 +2811,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>34</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>34</v>
       </c>
@@ -2845,7 +2845,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>34</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>34</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>34</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>34</v>
       </c>
@@ -2913,7 +2913,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>34</v>
       </c>
@@ -2930,7 +2930,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>34</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>34</v>
       </c>
@@ -2964,7 +2964,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>34</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>35</v>
       </c>
@@ -2998,7 +2998,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>35</v>
       </c>
@@ -3015,7 +3015,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>35</v>
       </c>
@@ -3032,7 +3032,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>35</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>35</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>35</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>35</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>35</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>35</v>
       </c>
@@ -3134,7 +3134,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>35</v>
       </c>
@@ -3151,7 +3151,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>35</v>
       </c>
@@ -3168,7 +3168,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>35</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>35</v>
       </c>
@@ -3202,7 +3202,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>35</v>
       </c>
@@ -3219,7 +3219,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>35</v>
       </c>
@@ -3236,7 +3236,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>35</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>35</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>35</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>35</v>
       </c>
@@ -3304,7 +3304,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>35</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>35</v>
       </c>
@@ -3338,7 +3338,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>35</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>35</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>35</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>35</v>
       </c>
@@ -3406,7 +3406,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>35</v>
       </c>
@@ -3423,7 +3423,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>35</v>
       </c>
@@ -3440,7 +3440,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>35</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>35</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>35</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>35</v>
       </c>
@@ -3508,7 +3508,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>35</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>35</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>35</v>
       </c>
@@ -3559,7 +3559,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>35</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>35</v>
       </c>
@@ -3593,7 +3593,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>35</v>
       </c>
@@ -3610,7 +3610,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>35</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>35</v>
       </c>
@@ -3644,7 +3644,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>35</v>
       </c>
@@ -3661,7 +3661,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>35</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>35</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>35</v>
       </c>
@@ -3712,7 +3712,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>35</v>
       </c>
@@ -3729,7 +3729,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>35</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>35</v>
       </c>
@@ -3763,7 +3763,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>35</v>
       </c>
@@ -3780,7 +3780,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>35</v>
       </c>
@@ -3797,7 +3797,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>36</v>
       </c>
@@ -3814,7 +3814,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>36</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>36</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>36</v>
       </c>
@@ -3865,7 +3865,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>36</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>36</v>
       </c>
@@ -3899,7 +3899,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>36</v>
       </c>
@@ -3916,7 +3916,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>36</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>36</v>
       </c>
@@ -3950,7 +3950,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>36</v>
       </c>
@@ -3967,7 +3967,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>36</v>
       </c>
@@ -3984,7 +3984,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>36</v>
       </c>
@@ -4001,7 +4001,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>36</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>36</v>
       </c>
@@ -4035,7 +4035,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>36</v>
       </c>
@@ -4052,7 +4052,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>36</v>
       </c>
@@ -4069,7 +4069,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>36</v>
       </c>
@@ -4086,7 +4086,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>36</v>
       </c>
@@ -4103,7 +4103,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>36</v>
       </c>
@@ -4120,7 +4120,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>36</v>
       </c>
@@ -4137,7 +4137,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>36</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>36</v>
       </c>
@@ -4171,7 +4171,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>36</v>
       </c>
@@ -4188,7 +4188,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>36</v>
       </c>
@@ -4205,7 +4205,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>36</v>
       </c>
@@ -4222,7 +4222,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>36</v>
       </c>
@@ -4239,7 +4239,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>36</v>
       </c>
@@ -4256,7 +4256,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>36</v>
       </c>
@@ -4273,7 +4273,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>36</v>
       </c>
@@ -4290,7 +4290,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>36</v>
       </c>
@@ -4307,7 +4307,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>36</v>
       </c>
@@ -4324,7 +4324,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>36</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>36</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>36</v>
       </c>
@@ -4375,7 +4375,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>36</v>
       </c>
@@ -4392,7 +4392,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>36</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>36</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>36</v>
       </c>
@@ -4443,7 +4443,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>36</v>
       </c>
@@ -4460,7 +4460,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>36</v>
       </c>
@@ -4477,7 +4477,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>36</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>36</v>
       </c>
@@ -4511,7 +4511,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>36</v>
       </c>
@@ -4528,7 +4528,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>36</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>36</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>36</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>36</v>
       </c>
@@ -4596,7 +4596,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>36</v>
       </c>
@@ -4613,7 +4613,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>37</v>
       </c>
@@ -4630,7 +4630,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>37</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>37</v>
       </c>
@@ -4664,7 +4664,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>37</v>
       </c>
@@ -4681,7 +4681,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>37</v>
       </c>
@@ -4698,7 +4698,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>37</v>
       </c>
@@ -4715,7 +4715,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>37</v>
       </c>
@@ -4732,7 +4732,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>37</v>
       </c>
@@ -4749,7 +4749,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>37</v>
       </c>
@@ -4766,7 +4766,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>37</v>
       </c>
@@ -4783,7 +4783,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>37</v>
       </c>
@@ -4800,7 +4800,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>37</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>37</v>
       </c>
@@ -4834,7 +4834,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>37</v>
       </c>
@@ -4851,7 +4851,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>37</v>
       </c>
@@ -4868,7 +4868,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>37</v>
       </c>
@@ -4885,7 +4885,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>37</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>37</v>
       </c>
@@ -4919,7 +4919,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>37</v>
       </c>
@@ -4936,7 +4936,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>37</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>37</v>
       </c>
@@ -4970,7 +4970,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>37</v>
       </c>
@@ -4987,7 +4987,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>37</v>
       </c>
@@ -5004,7 +5004,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>37</v>
       </c>
@@ -5021,7 +5021,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>37</v>
       </c>
@@ -5038,7 +5038,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>37</v>
       </c>
@@ -5055,7 +5055,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>37</v>
       </c>
@@ -5072,7 +5072,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>37</v>
       </c>
@@ -5089,7 +5089,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>37</v>
       </c>
@@ -5106,7 +5106,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>37</v>
       </c>
@@ -5123,7 +5123,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>37</v>
       </c>
@@ -5140,7 +5140,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>37</v>
       </c>
@@ -5157,7 +5157,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>37</v>
       </c>
@@ -5174,7 +5174,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>37</v>
       </c>
@@ -5191,7 +5191,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>37</v>
       </c>
@@ -5208,7 +5208,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>37</v>
       </c>
@@ -5225,7 +5225,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>37</v>
       </c>
@@ -5242,7 +5242,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>37</v>
       </c>
@@ -5259,7 +5259,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>37</v>
       </c>
@@ -5276,7 +5276,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>37</v>
       </c>
@@ -5293,7 +5293,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>37</v>
       </c>
@@ -5310,7 +5310,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>37</v>
       </c>
@@ -5327,7 +5327,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>37</v>
       </c>
@@ -5344,7 +5344,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>37</v>
       </c>
@@ -5361,7 +5361,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>37</v>
       </c>
@@ -5378,7 +5378,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>37</v>
       </c>
@@ -5395,7 +5395,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>37</v>
       </c>
@@ -5412,7 +5412,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>37</v>
       </c>
@@ -5429,7 +5429,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>38</v>
       </c>
@@ -5446,7 +5446,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>38</v>
       </c>
@@ -5463,7 +5463,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>38</v>
       </c>
@@ -5480,7 +5480,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>38</v>
       </c>
@@ -5497,7 +5497,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>38</v>
       </c>
@@ -5514,7 +5514,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>38</v>
       </c>
@@ -5531,7 +5531,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>38</v>
       </c>
@@ -5548,7 +5548,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>38</v>
       </c>
@@ -5565,7 +5565,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>38</v>
       </c>
@@ -5582,7 +5582,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>38</v>
       </c>
@@ -5599,7 +5599,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>38</v>
       </c>
@@ -5616,7 +5616,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>38</v>
       </c>
@@ -5633,7 +5633,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>38</v>
       </c>
@@ -5650,7 +5650,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>38</v>
       </c>
@@ -5667,7 +5667,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>38</v>
       </c>
@@ -5684,7 +5684,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>38</v>
       </c>
@@ -5701,7 +5701,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>38</v>
       </c>
@@ -5718,7 +5718,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>38</v>
       </c>
@@ -5735,7 +5735,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>38</v>
       </c>
@@ -5752,7 +5752,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>38</v>
       </c>
@@ -5769,7 +5769,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>38</v>
       </c>
@@ -5786,7 +5786,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>38</v>
       </c>
@@ -5803,7 +5803,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>38</v>
       </c>
@@ -5820,7 +5820,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>38</v>
       </c>
@@ -5837,7 +5837,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>38</v>
       </c>
@@ -5854,7 +5854,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>38</v>
       </c>
@@ -5871,7 +5871,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>38</v>
       </c>
@@ -5888,7 +5888,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>38</v>
       </c>
@@ -5905,7 +5905,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>38</v>
       </c>
@@ -5922,7 +5922,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>38</v>
       </c>
@@ -5939,7 +5939,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>38</v>
       </c>
@@ -5956,7 +5956,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>38</v>
       </c>
@@ -5973,7 +5973,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>38</v>
       </c>
@@ -5990,7 +5990,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>38</v>
       </c>
@@ -6007,7 +6007,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>38</v>
       </c>
@@ -6024,7 +6024,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>38</v>
       </c>
@@ -6041,7 +6041,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>38</v>
       </c>
@@ -6058,7 +6058,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>38</v>
       </c>
@@ -6075,7 +6075,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>38</v>
       </c>
@@ -6092,7 +6092,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>38</v>
       </c>
@@ -6109,7 +6109,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>38</v>
       </c>
@@ -6126,7 +6126,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>38</v>
       </c>
@@ -6143,7 +6143,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>38</v>
       </c>
@@ -6160,7 +6160,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>38</v>
       </c>
@@ -6177,7 +6177,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>38</v>
       </c>
@@ -6194,7 +6194,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>38</v>
       </c>
@@ -6211,7 +6211,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>38</v>
       </c>
@@ -6228,7 +6228,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>38</v>
       </c>
@@ -6245,7 +6245,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>39</v>
       </c>
@@ -6262,7 +6262,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>39</v>
       </c>
@@ -6279,7 +6279,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>39</v>
       </c>
@@ -6296,7 +6296,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>39</v>
       </c>
@@ -6313,7 +6313,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>39</v>
       </c>
@@ -6330,7 +6330,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>39</v>
       </c>
@@ -6347,7 +6347,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>39</v>
       </c>
@@ -6364,7 +6364,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>39</v>
       </c>
@@ -6381,7 +6381,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>39</v>
       </c>
@@ -6398,7 +6398,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>39</v>
       </c>
@@ -6415,7 +6415,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>39</v>
       </c>
@@ -6432,7 +6432,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>39</v>
       </c>
@@ -6449,7 +6449,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>39</v>
       </c>
@@ -6466,7 +6466,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>39</v>
       </c>
@@ -6483,7 +6483,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>39</v>
       </c>
@@ -6500,7 +6500,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>39</v>
       </c>
@@ -6517,7 +6517,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>39</v>
       </c>
@@ -6534,7 +6534,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
         <v>39</v>
       </c>
@@ -6551,7 +6551,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
         <v>39</v>
       </c>
@@ -6568,7 +6568,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>39</v>
       </c>
@@ -6585,7 +6585,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
         <v>39</v>
       </c>
@@ -6602,7 +6602,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>39</v>
       </c>
@@ -6619,7 +6619,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>39</v>
       </c>
@@ -6636,7 +6636,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>39</v>
       </c>
@@ -6653,7 +6653,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
         <v>39</v>
       </c>
@@ -6670,7 +6670,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
         <v>39</v>
       </c>
@@ -6687,7 +6687,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
         <v>39</v>
       </c>
@@ -6704,7 +6704,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
         <v>39</v>
       </c>
@@ -6721,7 +6721,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
         <v>39</v>
       </c>
@@ -6738,7 +6738,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
         <v>39</v>
       </c>
@@ -6755,7 +6755,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
         <v>39</v>
       </c>
@@ -6772,7 +6772,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>39</v>
       </c>
@@ -6789,7 +6789,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
         <v>39</v>
       </c>
@@ -6806,7 +6806,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
         <v>39</v>
       </c>
@@ -6823,7 +6823,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
         <v>39</v>
       </c>
@@ -6840,7 +6840,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>39</v>
       </c>
@@ -6857,7 +6857,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
         <v>39</v>
       </c>
@@ -6874,7 +6874,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
         <v>39</v>
       </c>
@@ -6891,7 +6891,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
         <v>39</v>
       </c>
@@ -6908,7 +6908,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>39</v>
       </c>
@@ -6925,7 +6925,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
         <v>39</v>
       </c>
@@ -6942,7 +6942,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
         <v>39</v>
       </c>
@@ -6959,7 +6959,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
         <v>39</v>
       </c>
@@ -6976,7 +6976,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="381" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
         <v>39</v>
       </c>
@@ -6993,7 +6993,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="382" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
         <v>39</v>
       </c>
@@ -7010,7 +7010,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="383" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
         <v>39</v>
       </c>
@@ -7027,7 +7027,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="384" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
         <v>39</v>
       </c>
@@ -7044,7 +7044,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="385" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
         <v>39</v>
       </c>
@@ -7061,7 +7061,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="386" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A386" t="s">
         <v>40</v>
       </c>
@@ -7078,7 +7078,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="387" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
         <v>40</v>
       </c>
@@ -7095,7 +7095,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="388" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
         <v>40</v>
       </c>
@@ -7112,7 +7112,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="389" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
         <v>40</v>
       </c>
@@ -7129,7 +7129,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="390" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
         <v>40</v>
       </c>
@@ -7146,7 +7146,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="391" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
         <v>40</v>
       </c>
@@ -7163,7 +7163,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="392" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
         <v>40</v>
       </c>
@@ -7180,7 +7180,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="393" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
         <v>40</v>
       </c>
@@ -7197,7 +7197,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="394" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
         <v>40</v>
       </c>
@@ -7214,7 +7214,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="395" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
         <v>40</v>
       </c>
@@ -7231,7 +7231,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="396" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
         <v>40</v>
       </c>
@@ -7248,7 +7248,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="397" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
         <v>40</v>
       </c>
@@ -7265,7 +7265,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="398" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
         <v>40</v>
       </c>
@@ -7282,7 +7282,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="399" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
         <v>40</v>
       </c>
@@ -7299,7 +7299,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="400" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
         <v>40</v>
       </c>
@@ -7316,7 +7316,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="401" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
         <v>40</v>
       </c>
@@ -7333,7 +7333,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="402" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
         <v>40</v>
       </c>
@@ -7350,7 +7350,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="403" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
         <v>40</v>
       </c>
@@ -7367,7 +7367,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="404" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
         <v>40</v>
       </c>
@@ -7384,7 +7384,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="405" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
         <v>40</v>
       </c>
@@ -7401,7 +7401,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="406" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
         <v>40</v>
       </c>
@@ -7418,7 +7418,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="407" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
         <v>40</v>
       </c>
@@ -7435,7 +7435,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="408" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
         <v>40</v>
       </c>
@@ -7452,7 +7452,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="409" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="409" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
         <v>40</v>
       </c>
@@ -7469,7 +7469,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="410" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="410" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A410" t="s">
         <v>40</v>
       </c>
@@ -7486,7 +7486,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="411" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="411" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
         <v>40</v>
       </c>
@@ -7503,7 +7503,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="412" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A412" t="s">
         <v>40</v>
       </c>
@@ -7520,7 +7520,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="413" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A413" t="s">
         <v>40</v>
       </c>
@@ -7537,7 +7537,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="414" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="414" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A414" t="s">
         <v>40</v>
       </c>
@@ -7554,7 +7554,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="415" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="415" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A415" t="s">
         <v>40</v>
       </c>
@@ -7571,7 +7571,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="416" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="416" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A416" t="s">
         <v>40</v>
       </c>
@@ -7588,7 +7588,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="417" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="417" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A417" t="s">
         <v>40</v>
       </c>
@@ -7605,7 +7605,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="418" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="418" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A418" t="s">
         <v>40</v>
       </c>
@@ -7622,7 +7622,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="419" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="419" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A419" t="s">
         <v>40</v>
       </c>
@@ -7639,7 +7639,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="420" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="420" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A420" t="s">
         <v>40</v>
       </c>
@@ -7656,7 +7656,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="421" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="421" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A421" t="s">
         <v>40</v>
       </c>
@@ -7673,7 +7673,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="422" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="422" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A422" t="s">
         <v>40</v>
       </c>
@@ -7690,7 +7690,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="423" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="423" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A423" t="s">
         <v>40</v>
       </c>
@@ -7707,7 +7707,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="424" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="424" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A424" t="s">
         <v>40</v>
       </c>
@@ -7724,7 +7724,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="425" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="425" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A425" t="s">
         <v>40</v>
       </c>
@@ -7741,7 +7741,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="426" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="426" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A426" t="s">
         <v>40</v>
       </c>
@@ -7758,7 +7758,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="427" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="427" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A427" t="s">
         <v>40</v>
       </c>
@@ -7775,7 +7775,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="428" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="428" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A428" t="s">
         <v>40</v>
       </c>
@@ -7792,7 +7792,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="429" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="429" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A429" t="s">
         <v>40</v>
       </c>
@@ -7809,7 +7809,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="430" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="430" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A430" t="s">
         <v>40</v>
       </c>
@@ -7826,7 +7826,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="431" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="431" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A431" t="s">
         <v>40</v>
       </c>
@@ -7843,7 +7843,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="432" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="432" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A432" t="s">
         <v>40</v>
       </c>
@@ -7860,7 +7860,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="433" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="433" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A433" t="s">
         <v>40</v>
       </c>
@@ -7877,7 +7877,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="434" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="434" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A434" t="s">
         <v>41</v>
       </c>
@@ -7894,7 +7894,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="435" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="435" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A435" t="s">
         <v>41</v>
       </c>
@@ -7911,7 +7911,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="436" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="436" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A436" t="s">
         <v>41</v>
       </c>
@@ -7928,7 +7928,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="437" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="437" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A437" t="s">
         <v>41</v>
       </c>
@@ -7945,7 +7945,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="438" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="438" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A438" t="s">
         <v>41</v>
       </c>
@@ -7962,7 +7962,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="439" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="439" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A439" t="s">
         <v>41</v>
       </c>
@@ -7979,7 +7979,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="440" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="440" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A440" t="s">
         <v>41</v>
       </c>
@@ -7996,7 +7996,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="441" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="441" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A441" t="s">
         <v>41</v>
       </c>
@@ -8013,7 +8013,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="442" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="442" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A442" t="s">
         <v>41</v>
       </c>
@@ -8030,7 +8030,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="443" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="443" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A443" t="s">
         <v>41</v>
       </c>
@@ -8047,7 +8047,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="444" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="444" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A444" t="s">
         <v>41</v>
       </c>
@@ -8064,7 +8064,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="445" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="445" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A445" t="s">
         <v>41</v>
       </c>
@@ -8081,7 +8081,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="446" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="446" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A446" t="s">
         <v>41</v>
       </c>
@@ -8098,7 +8098,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="447" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="447" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A447" t="s">
         <v>41</v>
       </c>
@@ -8115,7 +8115,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="448" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="448" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A448" t="s">
         <v>41</v>
       </c>
@@ -8132,7 +8132,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="449" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="449" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A449" t="s">
         <v>41</v>
       </c>
@@ -8149,7 +8149,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="450" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="450" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A450" t="s">
         <v>41</v>
       </c>
@@ -8166,7 +8166,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="451" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="451" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A451" t="s">
         <v>41</v>
       </c>
@@ -8183,7 +8183,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="452" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="452" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A452" t="s">
         <v>41</v>
       </c>
@@ -8200,7 +8200,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="453" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="453" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A453" t="s">
         <v>41</v>
       </c>
@@ -8217,7 +8217,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="454" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="454" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A454" t="s">
         <v>41</v>
       </c>
@@ -8234,7 +8234,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="455" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="455" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A455" t="s">
         <v>41</v>
       </c>
@@ -8251,7 +8251,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="456" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="456" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A456" t="s">
         <v>41</v>
       </c>
@@ -8268,7 +8268,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="457" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="457" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A457" t="s">
         <v>41</v>
       </c>
@@ -8285,7 +8285,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="458" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="458" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A458" t="s">
         <v>41</v>
       </c>
@@ -8302,7 +8302,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="459" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="459" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A459" t="s">
         <v>41</v>
       </c>
@@ -8319,7 +8319,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="460" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="460" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A460" t="s">
         <v>41</v>
       </c>
@@ -8336,7 +8336,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="461" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="461" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A461" t="s">
         <v>41</v>
       </c>
@@ -8353,7 +8353,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="462" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="462" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A462" t="s">
         <v>41</v>
       </c>
@@ -8370,7 +8370,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="463" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="463" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A463" t="s">
         <v>41</v>
       </c>
@@ -8387,7 +8387,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="464" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="464" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A464" t="s">
         <v>41</v>
       </c>
@@ -8404,7 +8404,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="465" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="465" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A465" t="s">
         <v>41</v>
       </c>
@@ -8421,7 +8421,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="466" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="466" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A466" t="s">
         <v>41</v>
       </c>
@@ -8438,7 +8438,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="467" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="467" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A467" t="s">
         <v>41</v>
       </c>
@@ -8455,7 +8455,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="468" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="468" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A468" t="s">
         <v>41</v>
       </c>
@@ -8472,7 +8472,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="469" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="469" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A469" t="s">
         <v>41</v>
       </c>
@@ -8489,7 +8489,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="470" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="470" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A470" t="s">
         <v>41</v>
       </c>
@@ -8506,7 +8506,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="471" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="471" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A471" t="s">
         <v>41</v>
       </c>
@@ -8523,7 +8523,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="472" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="472" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A472" t="s">
         <v>41</v>
       </c>
@@ -8540,7 +8540,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="473" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="473" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A473" t="s">
         <v>41</v>
       </c>
@@ -8557,7 +8557,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="474" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="474" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A474" t="s">
         <v>41</v>
       </c>
@@ -8574,7 +8574,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="475" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="475" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A475" t="s">
         <v>41</v>
       </c>
@@ -8591,7 +8591,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="476" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="476" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A476" t="s">
         <v>41</v>
       </c>
@@ -8608,7 +8608,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="477" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="477" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A477" t="s">
         <v>41</v>
       </c>
@@ -8625,7 +8625,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="478" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="478" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A478" t="s">
         <v>41</v>
       </c>
@@ -8642,7 +8642,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="479" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="479" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A479" t="s">
         <v>41</v>
       </c>
@@ -8659,7 +8659,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="480" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="480" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A480" t="s">
         <v>41</v>
       </c>
@@ -8676,7 +8676,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="481" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="481" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A481" t="s">
         <v>41</v>
       </c>

</xml_diff>